<commit_message>
Change dupage Tyler court to `dupage`
It's no longer `dupageinteg`, just `dupage`, on both stage and prod.
</commit_message>
<xml_diff>
--- a/docassemble/ILAOEfile/data/sources/il_courts.xlsx
+++ b/docassemble/ILAOEfile/data/sources/il_courts.xlsx
@@ -643,7 +643,7 @@
     <t xml:space="preserve">https://www.dupageco.org/courts/</t>
   </si>
   <si>
-    <t xml:space="preserve">dupageinteg</t>
+    <t xml:space="preserve">dupage</t>
   </si>
   <si>
     <t xml:space="preserve">Edgar County Courthouse</t>
@@ -2414,12 +2414,12 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="Q26" activeCellId="0" sqref="Q26"/>
+      <selection pane="bottomLeft" activeCell="S36" activeCellId="0" sqref="S36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.86"/>

</xml_diff>